<commit_message>
Add method to Board: food ordered by distance
</commit_message>
<xml_diff>
--- a/tests/sample_request.xlsx
+++ b/tests/sample_request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIOR03\DEV\battle-python\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDF3E5-9658-419B-B55C-1F602FD6B6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1124EC44-59AF-47DF-80E4-2BEFA26FFE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF568A77-CD93-4BC5-8ADF-5BB191CC88ED}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A2:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="7"/>
       <c r="H10" s="6" t="s">

</xml_diff>